<commit_message>
Ajout Du label et modif lien git
</commit_message>
<xml_diff>
--- a/zAutre Fichiers/Diagramme état transition matriciel.xlsx
+++ b/zAutre Fichiers/Diagramme état transition matriciel.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edouard\OneDrive - IUT de Bayonne\Bureau\SAE\S2.01\LecteurDiaporama\zAutre Fichiers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0E6B5DD5-C2E1-4FFD-B835-390B8A421C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17305AE2-E156-4532-B553-EAE177B58026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Ouvrir à propos</t>
   </si>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -463,22 +463,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="50.6640625" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="38.77734375" customWidth="1"/>
     <col min="4" max="4" width="15.88671875" customWidth="1"/>
     <col min="5" max="5" width="12.5546875" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" customWidth="1"/>
     <col min="7" max="7" width="17.109375" customWidth="1"/>
-    <col min="8" max="8" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="31.44140625" customWidth="1"/>
     <col min="9" max="9" width="28.21875" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
     <col min="11" max="11" width="39.109375" customWidth="1"/>
@@ -494,54 +495,30 @@
     <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
@@ -722,9 +699,7 @@
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A10" s="2"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -744,9 +719,7 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A11" s="2"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -766,9 +739,7 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -788,9 +759,7 @@
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -810,9 +779,7 @@
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A14" s="2"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -832,9 +799,7 @@
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>13</v>
-      </c>
+      <c r="A15" s="2"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -854,9 +819,7 @@
       <c r="R15" s="1"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="A16" s="2"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -876,9 +839,7 @@
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A17" s="2"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
@@ -898,9 +859,7 @@
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="A18" s="2"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>

</xml_diff>